<commit_message>
add new column called "Cek role"
</commit_message>
<xml_diff>
--- a/kuisoner.xlsx
+++ b/kuisoner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insidemedia-my.sharepoint.com/personal/hendra_respati_mindshareworld_com/Documents/Documents/GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hendra.respati\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{868FE46A-3779-4FD2-92ED-95BFAAB67988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1F4187-289B-4780-A3D0-9A4B960E2F16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Type Questionaire</t>
   </si>
@@ -87,12 +87,15 @@
   </si>
   <si>
     <t>Christofer.Yusalfino@mindshareworld.com</t>
+  </si>
+  <si>
+    <t>Cek role</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,114 +508,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -622,6 +633,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010061BDB6B1ABB82049809E76D71BC884B2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fcf29be6efcee6b9ffe6f94a122681c8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a90a6bd0-cf7d-4553-a7db-0d839a363391" xmlns:ns4="f96d9264-e323-4a54-ba03-d1f3c690c979" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52c74aaa3d0539db83ca8e1c1e31f7b5" ns3:_="" ns4:_="">
     <xsd:import namespace="a90a6bd0-cf7d-4553-a7db-0d839a363391"/>
@@ -844,22 +870,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEBA5599-0DDC-4DE6-9AFD-5941F0E638D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7001A4B7-D3F3-4929-8823-3BAC71038207}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC74B96F-AB84-4FA7-B314-E3D03C75CA37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -876,21 +904,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7001A4B7-D3F3-4929-8823-3BAC71038207}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEBA5599-0DDC-4DE6-9AFD-5941F0E638D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>